<commit_message>
Saving and Monitor improvement
Possibility to create and save several story in different xls sheet in
the same file
possibility to give limits to the cells to read
implemented a monitor to show user actions
</commit_message>
<xml_diff>
--- a/data/prova.xlsx
+++ b/data/prova.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr/>
+  <s:workbookPr codeName="ThisWorkbook"/>
   <s:bookViews>
     <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <s:sheet name="result" sheetId="2" r:id="rId2"/>
+    <s:sheet name="result_2" sheetId="2" r:id="rId2"/>
+    <s:sheet name="result_1" sheetId="3" r:id="rId3"/>
+    <s:sheet name="monza_100" sheetId="4" r:id="rId4"/>
+    <s:sheet name="monza_75" sheetId="5" r:id="rId5"/>
+    <s:sheet name="monza_50" sheetId="6" r:id="rId6"/>
+    <s:sheet name="monza_501" sheetId="7" r:id="rId7"/>
+    <s:sheet name="paul_100" sheetId="8" r:id="rId8"/>
+    <s:sheet name="barca_100" sheetId="9" r:id="rId9"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -378,7 +385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -399,200 +406,1488 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="n">
-        <v>61.8743</v>
+        <v>60.4687</v>
       </c>
       <c r="B2" t="n">
         <v>0.5</v>
       </c>
       <c r="C2" t="n">
-        <v>763.6745</v>
+        <v>1171.7892</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="n">
-        <v>38.7836</v>
+        <v>37.5874</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>752.1291</v>
+        <v>1167.1797</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="n">
-        <v>36.8895</v>
+        <v>30.3438</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>764.9085</v>
+        <v>1167.5936</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="n">
-        <v>31.4535</v>
+        <v>25.4523</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C5" t="n">
-        <v>758.1950000000001</v>
+        <v>1189.2975</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="n">
-        <v>31.3282</v>
+        <v>22.2781</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>755.8568</v>
+        <v>1156.1345</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="n">
-        <v>29.7975</v>
+        <v>19.1735</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C7" t="n">
-        <v>762.1809</v>
+        <v>1151.1416</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="n">
-        <v>26.1376</v>
+        <v>16.6059</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>771.9728</v>
+        <v>1183.7823</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="n">
-        <v>25.1335</v>
+        <v>13.0993</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C9" t="n">
-        <v>767.4165</v>
+        <v>1183.121</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="n">
-        <v>22.2421</v>
+        <v>12.5481</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>755.4511</v>
+        <v>1161.1956</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="n">
-        <v>20.724</v>
+        <v>11.1685</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>784.2496</v>
+        <v>1148.8189</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="n">
-        <v>20.032</v>
+        <v>8.4948</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C12" t="n">
-        <v>766.3641</v>
+        <v>1156.481</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="n">
-        <v>19.0249</v>
+        <v>5.2046</v>
       </c>
       <c r="B13" t="n">
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>755.0112</v>
+        <v>1182.7942</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="n">
-        <v>16.5364</v>
+        <v>3.6088</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C14" t="n">
-        <v>748.9233</v>
+        <v>1187.8662</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="n">
-        <v>14.7361</v>
+        <v>3.3754</v>
       </c>
       <c r="B15" t="n">
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>759.6532999999999</v>
+        <v>1147.8555</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="n">
-        <v>11.4518</v>
+        <v>0.4249</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>745.9186</v>
+        <v>1175.7854</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="n">
-        <v>5.5451</v>
+        <v>0.3474</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>748.8491</v>
+        <v>1172.5729</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="n">
-        <v>0.4604</v>
+        <v>0.0292</v>
       </c>
       <c r="B18" t="n">
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>766.3966</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="n">
-        <v>0.2058</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="n">
-        <v>765.0607</v>
+        <v>1156.0359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>60.4687</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1171.7892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>37.5874</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1167.1797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>30.3438</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1167.5936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
+        <v>25.4523</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1189.2975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
+        <v>22.2781</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1156.1345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
+        <v>19.1735</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1151.1416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="n">
+        <v>16.6059</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1183.7823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="n">
+        <v>13.0993</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1183.121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="n">
+        <v>12.5481</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1161.1956</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="n">
+        <v>11.1685</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1148.8189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="n">
+        <v>8.4948</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1156.481</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="n">
+        <v>5.2046</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1182.7942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="n">
+        <v>3.6088</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1187.8662</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="n">
+        <v>3.3754</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1147.8555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="n">
+        <v>0.4249</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1175.7854</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="n">
+        <v>0.3474</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1172.5729</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1156.0359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>60.4687</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1171.7892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>37.5874</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1167.1797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>30.3438</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1167.5936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
+        <v>25.4523</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1189.2975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
+        <v>22.2781</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1156.1345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
+        <v>19.1735</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1151.1416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="n">
+        <v>16.6059</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1183.7823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="n">
+        <v>13.0993</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1183.121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="n">
+        <v>12.5481</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1161.1956</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="n">
+        <v>11.1685</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1148.8189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="n">
+        <v>8.4948</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1156.481</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="n">
+        <v>5.2046</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1182.7942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="n">
+        <v>3.6088</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1187.8662</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="n">
+        <v>3.3754</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1147.8555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="n">
+        <v>0.4249</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1175.7854</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="n">
+        <v>0.3474</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1172.5729</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1156.0359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>44.4185</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1163.7641</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>37.5874</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1167.1797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>34.1309</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1165.4515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
+        <v>30.3438</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1167.5936</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
+        <v>22.2781</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1156.1345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
+        <v>19.1735</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1151.1416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="n">
+        <v>12.5481</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1161.1956</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="n">
+        <v>11.1685</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1148.8189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="n">
+        <v>8.4948</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1156.481</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="n">
+        <v>3.3754</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1147.8555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="n">
+        <v>0.4249</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1175.7854</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="n">
+        <v>0.3474</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1172.5729</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1156.0359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>41.2106</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1162.1602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>30.3438</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1167.5936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>22.2781</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1156.1345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
+        <v>19.1735</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1151.1416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
+        <v>12.5481</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1161.1956</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
+        <v>11.1685</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1148.8189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="n">
+        <v>8.4948</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1156.481</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="n">
+        <v>3.3754</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1147.8555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1156.0359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>41.2106</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1162.1602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>30.3438</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1167.5936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>22.2781</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1156.1345</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
+        <v>19.1735</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1151.1416</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
+        <v>12.5481</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1161.1956</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
+        <v>11.1685</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1148.8189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="n">
+        <v>8.4948</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1156.481</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="n">
+        <v>3.3754</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1147.8555</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1156.0359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>60.4687</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1171.7892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>37.5874</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1167.1797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>30.3438</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1167.5936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
+        <v>25.4523</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1189.2975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
+        <v>22.2781</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1156.1345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
+        <v>19.1735</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1151.1416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="n">
+        <v>16.6059</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1183.7823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="n">
+        <v>13.0993</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1183.121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="n">
+        <v>12.5481</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1161.1956</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="n">
+        <v>11.1685</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1148.8189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="n">
+        <v>8.4948</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1156.481</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="n">
+        <v>5.2046</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1182.7942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="n">
+        <v>3.6088</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1187.8662</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="n">
+        <v>3.3754</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1147.8555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="n">
+        <v>0.4249</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1175.7854</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="n">
+        <v>0.3474</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1172.5729</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1156.0359</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="n">
+        <v>60.4687</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1171.7892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="n">
+        <v>37.5874</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1167.1797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="n">
+        <v>30.3438</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1167.5936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="n">
+        <v>25.4523</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1189.2975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="n">
+        <v>22.2781</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1156.1345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="n">
+        <v>19.1735</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1151.1416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="n">
+        <v>16.6059</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1183.7823</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="n">
+        <v>13.0993</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1183.121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="n">
+        <v>12.5481</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1161.1956</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="n">
+        <v>11.1685</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1148.8189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="n">
+        <v>8.4948</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1156.481</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="n">
+        <v>5.2046</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1182.7942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="n">
+        <v>3.6088</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1187.8662</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="n">
+        <v>3.3754</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1147.8555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="n">
+        <v>0.4249</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1175.7854</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="n">
+        <v>0.3474</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1172.5729</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1156.0359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>